<commit_message>
Fixed toolbar appium issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Toolbar_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Toolbar_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -395,66 +395,6 @@
 ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
 PushConfigxml;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(toolbar_test_link);
-validate2;
-SelectTestToRun(VT283_0120_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-TakeScreenshot(VT283_0120);
-validate4;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0120_log_xpath);
-validate5;
-wait(2);
-press_Key(Back);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0120_Fullscreen_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-TakeScreenshot(Toolbar_Fullscreen);
-validate6;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0120_minimize_xpath);
-validate7;
-wait(2);
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Native Toolbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT283-0120
-};
-validate4
-{
-validate_Screenshot=VT283_0120
-};
-validate5
-{
-validate_Button_Exists=VT283_0120_Send_xpath
-};
-validate6
-{
-validate_Screenshot=Toolbar_Fullscreen
-};
-validate7
-{
-validate_AppMinimized=appsscreen
-};
-</t>
   </si>
   <si>
     <t>wait(3);
@@ -541,104 +481,6 @@
 };</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(toolbar_test_link);
-validate2;
-SelectTestToRun(VT283_0101_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-TakeScreenshot(VT283_0101);
-validate4;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0101_home_xpath);
-SwitchApp(WEBVIEW);
-TakeScreenshot(VT283_0101_home);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0101_refresh_xpath);
-SwitchApp(WEBVIEW);
-TakeScreenshot(VT283_0101_refresh);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0101_exit_xpath);
-validate5;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Native Toolbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT283-0101
-};
-validate4
-{
-validate_Screenshot=VT283_0101
-};
-validate5
-{
-validate_Screenshot=VT283_0101_home
-validate_Screenshot=VT283_0101_refresh
-validate_AppMinimized=appsscreen
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Native Toolbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT283-0102
-};
-validate4
-{
-validate_Screenshot=VT283_0102
-};
-validate5
-{
-validate_Screenshot=VT283_0102_back
-validate_Screenshot=VT283_0102_home
-validate_AppMinimized=appsscreen
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(toolbar_test_link);
-validate2;
-SelectTestToRun(VT283_0102_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-TakeScreenshot(VT283_0102);
-validate4;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(Toolbar_back_xpath);
-TakeScreenshot(VT283_0102_back);
-SwitchApp(WEBVIEW);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0102_103_home_xpath);
-SwitchApp(WEBVIEW);
-TakeScreenshot(VT283_0102_home);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0102_103_exit_xpath);
-validate5;
-</t>
-  </si>
-  <si>
     <t>wait(5);
 validate1;
 link_Click(toolbar_test_link);
@@ -672,54 +514,6 @@
 validate_Screenshot=VT283_0103
 };
 validate5
-{
-validate_AppMinimized=appsscreen
-};</t>
-  </si>
-  <si>
-    <t>wait(5);
-validate1;
-link_Click(toolbar_test_link);
-validate2;
-SelectTestToRun(VT283_0118_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-TakeScreenshot(VT283_0118);
-validate4;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0118_refresh_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-validate5;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT283_0118_exit_xpath);
-wait(2);
-validate6;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Native Toolbar JS Test
-};
-validate3
-{
-validate_Text_Exists=VT283-0118
-};
-validate4
-{
-validate_Screenshot=VT283_0118
-};
-validate5
-{
-validate_PageTitle=Native Toolbar JS Test
-};
-validate6
 {
 validate_AppMinimized=appsscreen
 };</t>
@@ -806,6 +600,158 @@
 validate_isIconDisplayed=EBtoobarview_xpath,false
 };
 </t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Native Toolbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT283-0101
+};
+validate4
+{
+validate_Screenshot=VT283_0101
+};
+validate5
+{
+validate_AppMinimized=appsscreen
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(toolbar_test_link);
+validate2;
+SelectTestToRun(VT283_0101_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeScreenshot(VT283_0101);
+validate4;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0101_home_xpath);
+SwitchApp(WEBVIEW);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0101_refresh_xpath);
+SwitchApp(WEBVIEW);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0101_exit_xpath);
+validate5;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Native Toolbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT283-0120
+};
+validate4
+{
+validate_Screenshot=VT283_0120
+};
+validate5
+{
+validate_Button_Exists=VT283_0120_Send_xpath
+};
+validate6
+{
+validate_fullscreen=webview_xpath,true
+};
+validate7
+{
+validate_AppMinimized=appsscreen
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(toolbar_test_link);
+validate2;
+SelectTestToRun(VT283_0120_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeScreenshot(VT283_0120);
+validate4;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0120_log_xpath);
+validate5;
+wait(2);
+press_Key(Back);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0120_Fullscreen_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+validate6;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0120_minimize_xpath);
+validate7;
+wait(2);
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+validate1;
+link_Click(toolbar_test_link);
+validate2;
+SelectTestToRun(VT283_0102_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeScreenshot(VT283_0102);
+validate4;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(Toolbar_back_xpath);
+SwitchApp(WEBVIEW);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0102_103_home_xpath);
+SwitchApp(WEBVIEW);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT283_0102_103_exit_xpath);
+validate5;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Native Toolbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT283-0102
+};
+validate4
+{
+validate_Screenshot=VT283_0102
+};
+validate5
+{
+validate_AppMinimized=appsscreen
+};</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1277,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1408,7 +1354,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="294" thickBot="1">
+    <row r="3" spans="1:11" ht="281.25" thickBot="1">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -1426,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="2"/>
@@ -1453,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -1480,10 +1426,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -1510,14 +1456,14 @@
         <v>56</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="230.25" thickBot="1">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -1544,7 +1490,7 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="306.75" thickBot="1">
-      <c r="A8" s="18">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -1561,17 +1507,17 @@
         <v>1</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="204.75" thickBot="1">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -1598,7 +1544,7 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="370.5" thickBot="1">
-      <c r="A10" s="18">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -1615,10 +1561,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -1651,86 +1597,59 @@
       <c r="J11" s="13"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="306.75" thickBot="1">
+    <row r="12" spans="1:11" ht="370.5" thickBot="1">
       <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1"/>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="E12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="15">
         <v>1</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="370.5" thickBot="1">
+      <c r="H12" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" ht="255.75" thickBot="1">
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="14">
-        <v>1</v>
-      </c>
-      <c r="C13" s="14"/>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="15">
-        <v>1</v>
-      </c>
-      <c r="G13" s="15" t="s">
+      <c r="E13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" ht="255.75" thickBot="1">
-      <c r="A14" s="18">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="2"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>